<commit_message>
Test data added to excel file.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milan GIIT\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LEARNING\SeleniumWorkspaces\SeleniumBasicConcepts\BasicSeleniumMVN\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{437D0B1E-B387-45B4-B3A9-9F6F5698AE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233DCA81-2356-4270-8ED1-E1170341E889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{88C90654-0B30-49B3-8241-18D30253E428}"/>
   </bookViews>
@@ -35,9 +35,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login with valid credentials.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +71,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +118,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +441,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A72401-27F4-4611-B7B7-1BEA1A8DDBAC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>